<commit_message>
updates to October 2023 data
</commit_message>
<xml_diff>
--- a/LIS/CTD/LISOct2023CastData.xlsx
+++ b/LIS/CTD/LISOct2023CastData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ccm21008\Documents\GitHub\gbl_matlab_tools\LIS\CTD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D534C3B1-6DE4-4601-8542-4088495AD582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C3616C-01AF-47FC-B368-A72F45DFA5FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27180" yWindow="3480" windowWidth="25335" windowHeight="12975" xr2:uid="{9ABC157E-A263-43E5-9437-64F4B0708557}"/>
+    <workbookView xWindow="1065" yWindow="1995" windowWidth="26475" windowHeight="13590" xr2:uid="{9ABC157E-A263-43E5-9437-64F4B0708557}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -251,9 +251,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -291,7 +291,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -397,7 +397,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -539,7 +539,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -550,7 +550,7 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>